<commit_message>
Add pictures Dec 2
</commit_message>
<xml_diff>
--- a/Source_Code/Data/000.xlsx
+++ b/Source_Code/Data/000.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5688" yWindow="0" windowWidth="16872" windowHeight="6384"/>
+    <workbookView xWindow="6624" yWindow="0" windowWidth="16872" windowHeight="6384"/>
   </bookViews>
   <sheets>
     <sheet name="000" sheetId="1" r:id="rId1"/>
@@ -33,27 +33,18 @@
     <t>tree moss</t>
   </si>
   <si>
-    <t>Dicranum  spp.</t>
-  </si>
-  <si>
     <t>dicranum mosses</t>
   </si>
   <si>
     <t>Hylocomium splendens</t>
   </si>
   <si>
-    <t>Mnium  spp.</t>
-  </si>
-  <si>
     <t>mnium mosses</t>
   </si>
   <si>
     <t>Pleurozium schreberi</t>
   </si>
   <si>
-    <t>Polytrichum  commune</t>
-  </si>
-  <si>
     <t>common hair-cap moss</t>
   </si>
   <si>
@@ -63,9 +54,6 @@
     <t>plume moss</t>
   </si>
   <si>
-    <t>Sphagnum  spp.</t>
-  </si>
-  <si>
     <t>sphagnum mosses</t>
   </si>
   <si>
@@ -81,15 +69,9 @@
     <t>hay-scented fern</t>
   </si>
   <si>
-    <t>Dryopteris  spp.</t>
-  </si>
-  <si>
     <t>wood ferns</t>
   </si>
   <si>
-    <t>Equisetum  spp.</t>
-  </si>
-  <si>
     <t>horsetails</t>
   </si>
   <si>
@@ -243,9 +225,6 @@
     <t>calypso orchid</t>
   </si>
   <si>
-    <t>Carex  spp.  – family only</t>
-  </si>
-  <si>
     <t>sedges</t>
   </si>
   <si>
@@ -315,9 +294,6 @@
     <t>wintergreen</t>
   </si>
   <si>
-    <t>Goodyera  spp.</t>
-  </si>
-  <si>
     <t>rattlesnake-plantains</t>
   </si>
   <si>
@@ -327,9 +303,6 @@
     <t>spotted touch-me-not</t>
   </si>
   <si>
-    <t>Juncus  spp.  – family only</t>
-  </si>
-  <si>
     <t>rushes</t>
   </si>
   <si>
@@ -345,9 +318,6 @@
     <t>twinflower</t>
   </si>
   <si>
-    <t>Lupinus  spp.</t>
-  </si>
-  <si>
     <t>lupins</t>
   </si>
   <si>
@@ -414,9 +384,6 @@
     <t>wood sorrel</t>
   </si>
   <si>
-    <t>Poaceae  –  family only</t>
-  </si>
-  <si>
     <t>grasses</t>
   </si>
   <si>
@@ -438,9 +405,6 @@
     <t>pitcher plant</t>
   </si>
   <si>
-    <t>Solidago  spp.</t>
-  </si>
-  <si>
     <t>goldenrods</t>
   </si>
   <si>
@@ -480,15 +444,9 @@
     <t>common speedwell</t>
   </si>
   <si>
-    <t>Vicia  spp.</t>
-  </si>
-  <si>
     <t>vetches</t>
   </si>
   <si>
-    <t>Viola  spp.</t>
-  </si>
-  <si>
     <t>violets</t>
   </si>
   <si>
@@ -510,9 +468,6 @@
     <t>lungwort</t>
   </si>
   <si>
-    <t>Usnea  spp.</t>
-  </si>
-  <si>
     <t>Acer spicatum</t>
   </si>
   <si>
@@ -531,9 +486,6 @@
     <t>green alder</t>
   </si>
   <si>
-    <t>Amelanchier  spp.</t>
-  </si>
-  <si>
     <t>serviceberries</t>
   </si>
   <si>
@@ -579,9 +531,6 @@
     <t>beaked hazel</t>
   </si>
   <si>
-    <t>Crataegus  spp.</t>
-  </si>
-  <si>
     <t>hawthorns</t>
   </si>
   <si>
@@ -702,9 +651,6 @@
     <t>bitter currant</t>
   </si>
   <si>
-    <t>Rosa  spp.</t>
-  </si>
-  <si>
     <t>wild roses</t>
   </si>
   <si>
@@ -718,9 +664,6 @@
   </si>
   <si>
     <t>wild red raspberry</t>
-  </si>
-  <si>
-    <t>Salix  spp.</t>
   </si>
   <si>
     <t>willows</t>
@@ -1831,6 +1774,63 @@
   <si>
     <t>lady slipper</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dicranum spp.</t>
+  </si>
+  <si>
+    <t>Mnium spp.</t>
+  </si>
+  <si>
+    <t>Polytrichum commune</t>
+  </si>
+  <si>
+    <t>Sphagnum spp.</t>
+  </si>
+  <si>
+    <t>Dryopteris spp.</t>
+  </si>
+  <si>
+    <t>Equisetum spp.</t>
+  </si>
+  <si>
+    <t>Carex spp. – family only</t>
+  </si>
+  <si>
+    <t>Goodyera spp.</t>
+  </si>
+  <si>
+    <t>Juncus spp. – family only</t>
+  </si>
+  <si>
+    <t>Lupinus spp.</t>
+  </si>
+  <si>
+    <t>Poaceae – family only</t>
+  </si>
+  <si>
+    <t>Solidago spp.</t>
+  </si>
+  <si>
+    <t>Vicia spp.</t>
+  </si>
+  <si>
+    <t>Viola spp.</t>
+  </si>
+  <si>
+    <t>Usnea spp.</t>
+  </si>
+  <si>
+    <t>Amelanchier spp.</t>
+  </si>
+  <si>
+    <t>Crataegus spp.</t>
+  </si>
+  <si>
+    <t>Rosa spp.</t>
+  </si>
+  <si>
+    <t>Salix spp.</t>
   </si>
 </sst>
 </file>
@@ -2787,8 +2787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2799,7 +2799,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>386</v>
+        <v>367</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2813,7 +2813,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>387</v>
+        <v>368</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -2827,13 +2827,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>388</v>
+        <v>369</v>
       </c>
       <c r="B3" t="s">
+        <v>581</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -2841,13 +2841,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>389</v>
+        <v>370</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>590</v>
+        <v>571</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2855,13 +2855,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>582</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -2869,13 +2869,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>591</v>
+        <v>572</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -2883,13 +2883,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>392</v>
+        <v>373</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>583</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -2897,13 +2897,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>393</v>
+        <v>374</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2911,13 +2911,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>394</v>
+        <v>375</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>584</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2925,13 +2925,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2939,13 +2939,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>396</v>
+        <v>377</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -2953,13 +2953,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>397</v>
+        <v>378</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>585</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2967,13 +2967,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>398</v>
+        <v>379</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>586</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2981,13 +2981,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>399</v>
+        <v>380</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2995,13 +2995,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>400</v>
+        <v>381</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3009,13 +3009,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>401</v>
+        <v>382</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -3023,13 +3023,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -3037,13 +3037,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>403</v>
+        <v>384</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -3051,13 +3051,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>404</v>
+        <v>385</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -3065,13 +3065,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -3079,13 +3079,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>406</v>
+        <v>387</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -3093,13 +3093,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>407</v>
+        <v>388</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -3107,13 +3107,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>408</v>
+        <v>389</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3121,13 +3121,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>409</v>
+        <v>390</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -3135,13 +3135,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>410</v>
+        <v>391</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -3149,13 +3149,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>411</v>
+        <v>392</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -3163,13 +3163,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>412</v>
+        <v>393</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -3177,13 +3177,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>413</v>
+        <v>394</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -3191,13 +3191,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>414</v>
+        <v>395</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -3205,13 +3205,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>415</v>
+        <v>396</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -3219,13 +3219,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>416</v>
+        <v>397</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -3233,13 +3233,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>417</v>
+        <v>398</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3247,13 +3247,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -3261,13 +3261,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -3275,13 +3275,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>420</v>
+        <v>401</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -3289,13 +3289,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>421</v>
+        <v>402</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -3303,13 +3303,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>422</v>
+        <v>403</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -3317,13 +3317,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>423</v>
+        <v>404</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -3331,13 +3331,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>587</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -3345,13 +3345,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>425</v>
+        <v>406</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -3359,13 +3359,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>426</v>
+        <v>407</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>589</v>
+        <v>570</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -3373,13 +3373,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>427</v>
+        <v>408</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C42" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -3387,13 +3387,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>428</v>
+        <v>409</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -3401,13 +3401,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>429</v>
+        <v>410</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -3415,13 +3415,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>599</v>
+        <v>580</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -3429,13 +3429,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>431</v>
+        <v>412</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C46" t="s">
-        <v>592</v>
+        <v>573</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -3443,13 +3443,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>432</v>
+        <v>413</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C47" t="s">
-        <v>587</v>
+        <v>568</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -3457,13 +3457,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>433</v>
+        <v>414</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -3471,13 +3471,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>434</v>
+        <v>415</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -3485,13 +3485,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>435</v>
+        <v>416</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C50" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -3499,13 +3499,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>436</v>
+        <v>417</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -3513,13 +3513,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>437</v>
+        <v>418</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C52" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -3527,13 +3527,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>438</v>
+        <v>419</v>
       </c>
       <c r="B53" t="s">
-        <v>98</v>
+        <v>588</v>
       </c>
       <c r="C53" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -3541,13 +3541,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>439</v>
+        <v>420</v>
       </c>
       <c r="B54" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C54" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -3555,13 +3555,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>440</v>
+        <v>421</v>
       </c>
       <c r="B55" t="s">
-        <v>102</v>
+        <v>589</v>
       </c>
       <c r="C55" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -3569,13 +3569,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>441</v>
+        <v>422</v>
       </c>
       <c r="B56" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -3583,13 +3583,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>442</v>
+        <v>423</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C57" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -3597,13 +3597,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>443</v>
+        <v>424</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
+        <v>590</v>
       </c>
       <c r="C58" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -3611,13 +3611,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>444</v>
+        <v>425</v>
       </c>
       <c r="B59" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C59" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -3625,13 +3625,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>445</v>
+        <v>426</v>
       </c>
       <c r="B60" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C60" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -3639,13 +3639,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>446</v>
+        <v>427</v>
       </c>
       <c r="B61" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C61" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -3653,13 +3653,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>447</v>
+        <v>428</v>
       </c>
       <c r="B62" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C62" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -3667,13 +3667,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>448</v>
+        <v>429</v>
       </c>
       <c r="B63" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C63" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -3681,13 +3681,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
       <c r="B64" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C64" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -3695,13 +3695,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>450</v>
+        <v>431</v>
       </c>
       <c r="B65" t="s">
-        <v>586</v>
+        <v>567</v>
       </c>
       <c r="C65" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -3709,13 +3709,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="B66" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C66" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -3723,13 +3723,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>452</v>
+        <v>433</v>
       </c>
       <c r="B67" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C67" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -3737,13 +3737,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
       <c r="B68" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C68" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -3751,13 +3751,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
       <c r="B69" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C69" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -3765,13 +3765,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>455</v>
+        <v>436</v>
       </c>
       <c r="B70" t="s">
-        <v>131</v>
+        <v>591</v>
       </c>
       <c r="C70" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -3779,13 +3779,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>456</v>
+        <v>437</v>
       </c>
       <c r="B71" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C71" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -3793,13 +3793,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="B72" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C72" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -3807,13 +3807,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>458</v>
+        <v>439</v>
       </c>
       <c r="B73" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C73" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -3821,13 +3821,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>459</v>
+        <v>440</v>
       </c>
       <c r="B74" t="s">
-        <v>139</v>
+        <v>592</v>
       </c>
       <c r="C74" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -3835,13 +3835,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>460</v>
+        <v>441</v>
       </c>
       <c r="B75" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C75" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -3849,13 +3849,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C76" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -3863,13 +3863,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="B77" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C77" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -3877,13 +3877,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>463</v>
+        <v>444</v>
       </c>
       <c r="B78" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C78" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -3891,13 +3891,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>464</v>
+        <v>445</v>
       </c>
       <c r="B79" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C79" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -3905,13 +3905,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>465</v>
+        <v>446</v>
       </c>
       <c r="B80" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C80" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -3919,13 +3919,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>466</v>
+        <v>447</v>
       </c>
       <c r="B81" t="s">
-        <v>153</v>
+        <v>593</v>
       </c>
       <c r="C81" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -3933,13 +3933,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>467</v>
+        <v>448</v>
       </c>
       <c r="B82" t="s">
-        <v>155</v>
+        <v>594</v>
       </c>
       <c r="C82" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -3947,13 +3947,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>468</v>
+        <v>449</v>
       </c>
       <c r="B83" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C83" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -3961,13 +3961,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>469</v>
+        <v>450</v>
       </c>
       <c r="B84" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C84" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -3975,13 +3975,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>470</v>
+        <v>451</v>
       </c>
       <c r="B85" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C85" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -3989,13 +3989,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>471</v>
+        <v>452</v>
       </c>
       <c r="B86" t="s">
-        <v>163</v>
+        <v>595</v>
       </c>
       <c r="C86" t="s">
-        <v>593</v>
+        <v>574</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -4003,13 +4003,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>472</v>
+        <v>453</v>
       </c>
       <c r="B87" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="C87" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -4017,13 +4017,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>473</v>
+        <v>454</v>
       </c>
       <c r="B88" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C88" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -4031,13 +4031,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>474</v>
+        <v>455</v>
       </c>
       <c r="B89" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="C89" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -4045,13 +4045,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>475</v>
+        <v>456</v>
       </c>
       <c r="B90" t="s">
-        <v>170</v>
+        <v>596</v>
       </c>
       <c r="C90" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -4059,13 +4059,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>476</v>
+        <v>457</v>
       </c>
       <c r="B91" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="C91" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -4073,13 +4073,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>477</v>
+        <v>458</v>
       </c>
       <c r="B92" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="C92" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -4087,13 +4087,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>478</v>
+        <v>459</v>
       </c>
       <c r="B93" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="C93" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -4101,13 +4101,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
       <c r="B94" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C94" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -4115,13 +4115,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>480</v>
+        <v>461</v>
       </c>
       <c r="B95" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C95" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -4129,13 +4129,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>481</v>
+        <v>462</v>
       </c>
       <c r="B96" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C96" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -4143,13 +4143,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>482</v>
+        <v>463</v>
       </c>
       <c r="B97" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="C97" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -4157,13 +4157,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>483</v>
+        <v>464</v>
       </c>
       <c r="B98" t="s">
-        <v>186</v>
+        <v>597</v>
       </c>
       <c r="C98" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -4171,13 +4171,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>484</v>
+        <v>465</v>
       </c>
       <c r="B99" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="C99" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -4185,13 +4185,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>485</v>
+        <v>466</v>
       </c>
       <c r="B100" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="C100" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -4199,13 +4199,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
       <c r="B101" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="C101" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -4213,13 +4213,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="B102" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="C102" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -4227,13 +4227,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
       <c r="B103" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="C103" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -4241,13 +4241,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>489</v>
+        <v>470</v>
       </c>
       <c r="B104" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="C104" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -4255,13 +4255,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>490</v>
+        <v>471</v>
       </c>
       <c r="B105" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="C105" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -4269,13 +4269,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>491</v>
+        <v>472</v>
       </c>
       <c r="B106" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="C106" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -4283,13 +4283,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>492</v>
+        <v>473</v>
       </c>
       <c r="B107" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="C107" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -4297,13 +4297,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>493</v>
+        <v>474</v>
       </c>
       <c r="B108" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="C108" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -4311,13 +4311,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>494</v>
+        <v>475</v>
       </c>
       <c r="B109" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="C109" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -4325,13 +4325,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>495</v>
+        <v>476</v>
       </c>
       <c r="B110" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="C110" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -4339,13 +4339,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>496</v>
+        <v>477</v>
       </c>
       <c r="B111" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="C111" t="s">
-        <v>588</v>
+        <v>569</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -4353,13 +4353,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>497</v>
+        <v>478</v>
       </c>
       <c r="B112" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="C112" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="D112">
         <v>1</v>
@@ -4367,13 +4367,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>498</v>
+        <v>479</v>
       </c>
       <c r="B113" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="C113" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="D113">
         <v>1</v>
@@ -4381,13 +4381,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>499</v>
+        <v>480</v>
       </c>
       <c r="B114" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="C114" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -4395,13 +4395,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>500</v>
+        <v>481</v>
       </c>
       <c r="B115" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="C115" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="D115">
         <v>1</v>
@@ -4409,13 +4409,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>501</v>
+        <v>482</v>
       </c>
       <c r="B116" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="C116" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -4423,13 +4423,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>502</v>
+        <v>483</v>
       </c>
       <c r="B117" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="C117" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D117">
         <v>1</v>
@@ -4437,13 +4437,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>503</v>
+        <v>484</v>
       </c>
       <c r="B118" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="C118" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -4451,13 +4451,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>504</v>
+        <v>485</v>
       </c>
       <c r="B119" t="s">
-        <v>227</v>
+        <v>598</v>
       </c>
       <c r="C119" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -4465,13 +4465,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>505</v>
+        <v>486</v>
       </c>
       <c r="B120" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="C120" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="D120">
         <v>0</v>
@@ -4479,13 +4479,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>506</v>
+        <v>487</v>
       </c>
       <c r="B121" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="C121" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -4493,13 +4493,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>507</v>
+        <v>488</v>
       </c>
       <c r="B122" t="s">
-        <v>233</v>
+        <v>599</v>
       </c>
       <c r="C122" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="D122">
         <v>0</v>
@@ -4507,13 +4507,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>508</v>
+        <v>489</v>
       </c>
       <c r="B123" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="C123" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -4521,13 +4521,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>509</v>
+        <v>490</v>
       </c>
       <c r="B124" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="C124" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -4535,13 +4535,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>510</v>
+        <v>491</v>
       </c>
       <c r="B125" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="C125" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="D125">
         <v>0</v>
@@ -4549,13 +4549,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>511</v>
+        <v>492</v>
       </c>
       <c r="B126" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="C126" t="s">
-        <v>598</v>
+        <v>579</v>
       </c>
       <c r="D126">
         <v>0</v>
@@ -4563,13 +4563,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>512</v>
+        <v>493</v>
       </c>
       <c r="B127" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="C127" t="s">
-        <v>597</v>
+        <v>578</v>
       </c>
       <c r="D127">
         <v>1</v>
@@ -4577,13 +4577,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>513</v>
+        <v>494</v>
       </c>
       <c r="B128" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="C128" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="D128">
         <v>0</v>
@@ -4591,13 +4591,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>514</v>
+        <v>495</v>
       </c>
       <c r="B129" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="C129" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="D129">
         <v>0</v>
@@ -4605,13 +4605,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>515</v>
+        <v>496</v>
       </c>
       <c r="B130" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="C130" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="D130">
         <v>1</v>
@@ -4619,13 +4619,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>516</v>
+        <v>497</v>
       </c>
       <c r="B131" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="C131" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="D131">
         <v>0</v>
@@ -4633,13 +4633,13 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>517</v>
+        <v>498</v>
       </c>
       <c r="B132" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="C132" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="D132">
         <v>0</v>
@@ -4647,13 +4647,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>518</v>
+        <v>499</v>
       </c>
       <c r="B133" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="C133" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="D133">
         <v>0</v>
@@ -4661,13 +4661,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>519</v>
+        <v>500</v>
       </c>
       <c r="B134" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="C134" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="D134">
         <v>0</v>
@@ -4675,13 +4675,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>520</v>
+        <v>501</v>
       </c>
       <c r="B135" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="C135" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="D135">
         <v>0</v>
@@ -4689,13 +4689,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>521</v>
+        <v>502</v>
       </c>
       <c r="B136" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="C136" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -4703,13 +4703,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>522</v>
+        <v>503</v>
       </c>
       <c r="B137" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="C137" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="D137">
         <v>0</v>
@@ -4717,13 +4717,13 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>523</v>
+        <v>504</v>
       </c>
       <c r="B138" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="C138" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="D138">
         <v>0</v>
@@ -4731,13 +4731,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>524</v>
+        <v>505</v>
       </c>
       <c r="B139" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="C139" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="D139">
         <v>0</v>
@@ -4745,13 +4745,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>525</v>
+        <v>506</v>
       </c>
       <c r="B140" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="C140" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="D140">
         <v>0</v>
@@ -4759,13 +4759,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>526</v>
+        <v>507</v>
       </c>
       <c r="B141" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
       <c r="C141" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="D141">
         <v>1</v>
@@ -4773,13 +4773,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>527</v>
+        <v>508</v>
       </c>
       <c r="B142" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="C142" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="D142">
         <v>0</v>
@@ -4787,13 +4787,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>528</v>
+        <v>509</v>
       </c>
       <c r="B143" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
       <c r="C143" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="D143">
         <v>1</v>
@@ -4801,13 +4801,13 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>529</v>
+        <v>510</v>
       </c>
       <c r="B144" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
       <c r="C144" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="D144">
         <v>1</v>
@@ -4815,13 +4815,13 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>530</v>
+        <v>511</v>
       </c>
       <c r="B145" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="C145" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="D145">
         <v>1</v>
@@ -4829,13 +4829,13 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>531</v>
+        <v>512</v>
       </c>
       <c r="B146" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="C146" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="D146">
         <v>0</v>
@@ -4843,13 +4843,13 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>532</v>
+        <v>513</v>
       </c>
       <c r="B147" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="C147" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="D147">
         <v>1</v>
@@ -4857,13 +4857,13 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>533</v>
+        <v>514</v>
       </c>
       <c r="B148" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="C148" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="D148">
         <v>1</v>
@@ -4871,13 +4871,13 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>534</v>
+        <v>515</v>
       </c>
       <c r="B149" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="C149" t="s">
-        <v>596</v>
+        <v>577</v>
       </c>
       <c r="D149">
         <v>1</v>
@@ -4885,13 +4885,13 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>535</v>
+        <v>516</v>
       </c>
       <c r="B150" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="C150" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="D150">
         <v>0</v>
@@ -4899,13 +4899,13 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>536</v>
+        <v>517</v>
       </c>
       <c r="B151" t="s">
-        <v>288</v>
+        <v>269</v>
       </c>
       <c r="C151" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="D151">
         <v>0</v>
@@ -4913,13 +4913,13 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>537</v>
+        <v>518</v>
       </c>
       <c r="B152" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="C152" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="D152">
         <v>1</v>
@@ -4927,13 +4927,13 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>538</v>
+        <v>519</v>
       </c>
       <c r="B153" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="C153" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="D153">
         <v>1</v>
@@ -4941,13 +4941,13 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>539</v>
+        <v>520</v>
       </c>
       <c r="B154" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="C154" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="D154">
         <v>1</v>
@@ -4955,13 +4955,13 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>540</v>
+        <v>521</v>
       </c>
       <c r="B155" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="C155" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="D155">
         <v>0</v>
@@ -4969,13 +4969,13 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>541</v>
+        <v>522</v>
       </c>
       <c r="B156" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="C156" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="D156">
         <v>1</v>
@@ -4983,13 +4983,13 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>542</v>
+        <v>523</v>
       </c>
       <c r="B157" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="C157" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
       <c r="D157">
         <v>0</v>
@@ -4997,13 +4997,13 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>543</v>
+        <v>524</v>
       </c>
       <c r="B158" t="s">
-        <v>302</v>
+        <v>283</v>
       </c>
       <c r="C158" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="D158">
         <v>0</v>
@@ -5011,13 +5011,13 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>544</v>
+        <v>525</v>
       </c>
       <c r="B159" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
       <c r="C159" t="s">
-        <v>305</v>
+        <v>286</v>
       </c>
       <c r="D159">
         <v>0</v>
@@ -5025,13 +5025,13 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>545</v>
+        <v>526</v>
       </c>
       <c r="B160" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="C160" t="s">
-        <v>595</v>
+        <v>576</v>
       </c>
       <c r="D160">
         <v>1</v>
@@ -5039,13 +5039,13 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>546</v>
+        <v>527</v>
       </c>
       <c r="B161" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="C161" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
       <c r="D161">
         <v>0</v>
@@ -5053,13 +5053,13 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>547</v>
+        <v>528</v>
       </c>
       <c r="B162" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="C162" t="s">
-        <v>310</v>
+        <v>291</v>
       </c>
       <c r="D162">
         <v>1</v>
@@ -5067,13 +5067,13 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>548</v>
+        <v>529</v>
       </c>
       <c r="B163" t="s">
-        <v>311</v>
+        <v>292</v>
       </c>
       <c r="C163" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="D163">
         <v>0</v>
@@ -5081,13 +5081,13 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>549</v>
+        <v>530</v>
       </c>
       <c r="B164" t="s">
-        <v>313</v>
+        <v>294</v>
       </c>
       <c r="C164" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
       <c r="D164">
         <v>1</v>
@@ -5095,13 +5095,13 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>550</v>
+        <v>531</v>
       </c>
       <c r="B165" t="s">
-        <v>315</v>
+        <v>296</v>
       </c>
       <c r="C165" t="s">
-        <v>316</v>
+        <v>297</v>
       </c>
       <c r="D165">
         <v>1</v>
@@ -5109,13 +5109,13 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>551</v>
+        <v>532</v>
       </c>
       <c r="B166" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="C166" t="s">
-        <v>318</v>
+        <v>299</v>
       </c>
       <c r="D166">
         <v>1</v>
@@ -5123,13 +5123,13 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>552</v>
+        <v>533</v>
       </c>
       <c r="B167" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="C167" t="s">
-        <v>320</v>
+        <v>301</v>
       </c>
       <c r="D167">
         <v>0</v>
@@ -5137,13 +5137,13 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>553</v>
+        <v>534</v>
       </c>
       <c r="B168" t="s">
-        <v>321</v>
+        <v>302</v>
       </c>
       <c r="C168" t="s">
-        <v>322</v>
+        <v>303</v>
       </c>
       <c r="D168">
         <v>1</v>
@@ -5151,13 +5151,13 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>554</v>
+        <v>535</v>
       </c>
       <c r="B169" t="s">
-        <v>323</v>
+        <v>304</v>
       </c>
       <c r="C169" t="s">
-        <v>324</v>
+        <v>305</v>
       </c>
       <c r="D169">
         <v>0</v>
@@ -5165,13 +5165,13 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>555</v>
+        <v>536</v>
       </c>
       <c r="B170" t="s">
-        <v>325</v>
+        <v>306</v>
       </c>
       <c r="C170" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="D170">
         <v>0</v>
@@ -5179,13 +5179,13 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>556</v>
+        <v>537</v>
       </c>
       <c r="B171" t="s">
-        <v>327</v>
+        <v>308</v>
       </c>
       <c r="C171" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="D171">
         <v>0</v>
@@ -5193,13 +5193,13 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>557</v>
+        <v>538</v>
       </c>
       <c r="B172" t="s">
-        <v>329</v>
+        <v>310</v>
       </c>
       <c r="C172" t="s">
-        <v>330</v>
+        <v>311</v>
       </c>
       <c r="D172">
         <v>0</v>
@@ -5207,13 +5207,13 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>558</v>
+        <v>539</v>
       </c>
       <c r="B173" t="s">
-        <v>331</v>
+        <v>312</v>
       </c>
       <c r="C173" t="s">
-        <v>332</v>
+        <v>313</v>
       </c>
       <c r="D173">
         <v>1</v>
@@ -5221,13 +5221,13 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>559</v>
+        <v>540</v>
       </c>
       <c r="B174" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="C174" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
       <c r="D174">
         <v>0</v>
@@ -5235,13 +5235,13 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>560</v>
+        <v>541</v>
       </c>
       <c r="B175" t="s">
-        <v>335</v>
+        <v>316</v>
       </c>
       <c r="C175" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="D175">
         <v>1</v>
@@ -5249,13 +5249,13 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>561</v>
+        <v>542</v>
       </c>
       <c r="B176" t="s">
-        <v>337</v>
+        <v>318</v>
       </c>
       <c r="C176" t="s">
-        <v>338</v>
+        <v>319</v>
       </c>
       <c r="D176">
         <v>0</v>
@@ -5263,13 +5263,13 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>562</v>
+        <v>543</v>
       </c>
       <c r="B177" t="s">
-        <v>339</v>
+        <v>320</v>
       </c>
       <c r="C177" t="s">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="D177">
         <v>0</v>
@@ -5277,13 +5277,13 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>563</v>
+        <v>544</v>
       </c>
       <c r="B178" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
       <c r="C178" t="s">
-        <v>342</v>
+        <v>323</v>
       </c>
       <c r="D178">
         <v>1</v>
@@ -5291,13 +5291,13 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>564</v>
+        <v>545</v>
       </c>
       <c r="B179" t="s">
-        <v>343</v>
+        <v>324</v>
       </c>
       <c r="C179" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="D179">
         <v>1</v>
@@ -5305,13 +5305,13 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>565</v>
+        <v>546</v>
       </c>
       <c r="B180" t="s">
-        <v>345</v>
+        <v>326</v>
       </c>
       <c r="C180" t="s">
-        <v>346</v>
+        <v>327</v>
       </c>
       <c r="D180">
         <v>0</v>
@@ -5319,13 +5319,13 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>566</v>
+        <v>547</v>
       </c>
       <c r="B181" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="C181" t="s">
-        <v>348</v>
+        <v>329</v>
       </c>
       <c r="D181">
         <v>1</v>
@@ -5333,13 +5333,13 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>567</v>
+        <v>548</v>
       </c>
       <c r="B182" t="s">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="C182" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
       <c r="D182">
         <v>0</v>
@@ -5347,13 +5347,13 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>568</v>
+        <v>549</v>
       </c>
       <c r="B183" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="C183" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
       <c r="D183">
         <v>1</v>
@@ -5361,13 +5361,13 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>569</v>
+        <v>550</v>
       </c>
       <c r="B184" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="C184" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="D184">
         <v>0</v>
@@ -5375,13 +5375,13 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>570</v>
+        <v>551</v>
       </c>
       <c r="B185" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="C185" t="s">
-        <v>356</v>
+        <v>337</v>
       </c>
       <c r="D185">
         <v>0</v>
@@ -5389,13 +5389,13 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>571</v>
+        <v>552</v>
       </c>
       <c r="B186" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="C186" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="D186">
         <v>0</v>
@@ -5403,13 +5403,13 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>572</v>
+        <v>553</v>
       </c>
       <c r="B187" t="s">
-        <v>359</v>
+        <v>340</v>
       </c>
       <c r="C187" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
       <c r="D187">
         <v>0</v>
@@ -5417,13 +5417,13 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>573</v>
+        <v>554</v>
       </c>
       <c r="B188" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="C188" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
       <c r="D188">
         <v>0</v>
@@ -5431,13 +5431,13 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>574</v>
+        <v>555</v>
       </c>
       <c r="B189" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
       <c r="C189" t="s">
-        <v>594</v>
+        <v>575</v>
       </c>
       <c r="D189">
         <v>0</v>
@@ -5445,13 +5445,13 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="B190" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
       <c r="C190" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
       <c r="D190">
         <v>1</v>
@@ -5459,13 +5459,13 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>576</v>
+        <v>557</v>
       </c>
       <c r="B191" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="C191" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="D191">
         <v>1</v>
@@ -5473,13 +5473,13 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>577</v>
+        <v>558</v>
       </c>
       <c r="B192" t="s">
-        <v>368</v>
+        <v>349</v>
       </c>
       <c r="C192" t="s">
-        <v>369</v>
+        <v>350</v>
       </c>
       <c r="D192">
         <v>1</v>
@@ -5487,13 +5487,13 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>578</v>
+        <v>559</v>
       </c>
       <c r="B193" t="s">
-        <v>370</v>
+        <v>351</v>
       </c>
       <c r="C193" t="s">
-        <v>371</v>
+        <v>352</v>
       </c>
       <c r="D193">
         <v>1</v>
@@ -5501,13 +5501,13 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>579</v>
+        <v>560</v>
       </c>
       <c r="B194" t="s">
-        <v>372</v>
+        <v>353</v>
       </c>
       <c r="C194" t="s">
-        <v>373</v>
+        <v>354</v>
       </c>
       <c r="D194">
         <v>0</v>
@@ -5515,13 +5515,13 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>580</v>
+        <v>561</v>
       </c>
       <c r="B195" t="s">
-        <v>374</v>
+        <v>355</v>
       </c>
       <c r="C195" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
       <c r="D195">
         <v>1</v>
@@ -5529,13 +5529,13 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>581</v>
+        <v>562</v>
       </c>
       <c r="B196" t="s">
-        <v>376</v>
+        <v>357</v>
       </c>
       <c r="C196" t="s">
-        <v>377</v>
+        <v>358</v>
       </c>
       <c r="D196">
         <v>0</v>
@@ -5543,13 +5543,13 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>582</v>
+        <v>563</v>
       </c>
       <c r="B197" t="s">
-        <v>378</v>
+        <v>359</v>
       </c>
       <c r="C197" t="s">
-        <v>379</v>
+        <v>360</v>
       </c>
       <c r="D197">
         <v>1</v>
@@ -5557,13 +5557,13 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>583</v>
+        <v>564</v>
       </c>
       <c r="B198" t="s">
-        <v>380</v>
+        <v>361</v>
       </c>
       <c r="C198" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
       <c r="D198">
         <v>0</v>
@@ -5571,13 +5571,13 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>584</v>
+        <v>565</v>
       </c>
       <c r="B199" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
       <c r="C199" t="s">
-        <v>383</v>
+        <v>364</v>
       </c>
       <c r="D199">
         <v>0</v>
@@ -5585,13 +5585,13 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>585</v>
+        <v>566</v>
       </c>
       <c r="B200" t="s">
-        <v>384</v>
+        <v>365</v>
       </c>
       <c r="C200" t="s">
-        <v>385</v>
+        <v>366</v>
       </c>
       <c r="D200">
         <v>1</v>

</xml_diff>